<commit_message>
update mono test last
</commit_message>
<xml_diff>
--- a/Test_mono2.xlsx
+++ b/Test_mono2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbgan\OneDrive\Desktop\WORK\Aj_Woot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074F53F-34BB-4B83-A08C-3C86DD513204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4290F06-222E-4B84-8041-08C6A0A7963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{29004776-18DE-466A-8025-2390A1832D06}"/>
   </bookViews>
@@ -2653,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F0A25E-BC79-46F4-BB6C-776B7465BF37}">
   <dimension ref="A1:AC297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D137" workbookViewId="0">
-      <selection activeCell="F295" sqref="F295"/>
+    <sheetView tabSelected="1" topLeftCell="F192" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -2669,7 +2669,7 @@
     <col min="9" max="9" width="11.42578125" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="5"/>
+    <col min="12" max="12" width="11.5703125" style="5" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="5"/>
     <col min="15" max="15" width="13.42578125" style="14" customWidth="1"/>
@@ -28185,14 +28185,14 @@
     </row>
     <row r="293" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F293" s="5">
-        <f>(0.006-0.01)*300+60.17</f>
-        <v>58.97</v>
+        <f>(0.065)*500+59.67</f>
+        <v>92.17</v>
       </c>
     </row>
     <row r="295" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F295" s="5">
-        <f>3.53/0.06</f>
-        <v>58.833333333333336</v>
+        <f>3.75/0.06</f>
+        <v>62.5</v>
       </c>
     </row>
     <row r="297" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>